<commit_message>
Poster ready, committing everything.
</commit_message>
<xml_diff>
--- a/figures/distributions.xlsx
+++ b/figures/distributions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="genders" sheetId="2" r:id="rId1"/>
@@ -155,11 +155,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="135428352"/>
-        <c:axId val="135446528"/>
+        <c:axId val="98080640"/>
+        <c:axId val="98082176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135428352"/>
+        <c:axId val="98080640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -168,7 +168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135446528"/>
+        <c:crossAx val="98082176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -176,7 +176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135446528"/>
+        <c:axId val="98082176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -187,7 +187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135428352"/>
+        <c:crossAx val="98080640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -371,11 +371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="14"/>
-        <c:axId val="136523136"/>
-        <c:axId val="136541696"/>
+        <c:axId val="98348416"/>
+        <c:axId val="98375168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136523136"/>
+        <c:axId val="98348416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -417,13 +417,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136541696"/>
+        <c:crossAx val="98375168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -432,7 +431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136541696"/>
+        <c:axId val="98375168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8000"/>
@@ -481,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136523136"/>
+        <c:crossAx val="98348416"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4000"/>
@@ -878,28 +877,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>21313</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>B2/SUM($B$2:$B$3)</f>
+        <v>0.44034214169128738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>27088</v>
+      </c>
+      <c r="C3">
+        <f>B3/SUM($B$2:$B$3)</f>
+        <v>0.55965785830871262</v>
       </c>
     </row>
   </sheetData>
@@ -912,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AF66" sqref="AF66"/>
     </sheetView>
   </sheetViews>

</xml_diff>